<commit_message>
Update Ultrasonic Sensor Test Results
</commit_message>
<xml_diff>
--- a/Documents/Ultrasonic Sensor Test Results.xlsx
+++ b/Documents/Ultrasonic Sensor Test Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Actual Distance(mm)</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>Error (mm)</t>
+  </si>
+  <si>
+    <t>Note* Beyond 1000mm, the distance appears to wrap, indicating a timer overflow.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If more than 1m distance required for the project, I'll have to look into timer overflow counting.</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +399,7 @@
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>20</v>
       </c>
@@ -415,8 +421,11 @@
         <f t="shared" ref="C2:C52" si="0">A2-B2</f>
         <v>-10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>30</v>
       </c>
@@ -427,8 +436,11 @@
         <f t="shared" si="0"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40</v>
       </c>
@@ -440,7 +452,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>50</v>
       </c>
@@ -452,7 +464,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>60</v>
       </c>
@@ -464,7 +476,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>70</v>
       </c>
@@ -476,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>80</v>
       </c>
@@ -488,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>90</v>
       </c>
@@ -500,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>100</v>
       </c>
@@ -512,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>110</v>
       </c>
@@ -524,7 +536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>120</v>
       </c>
@@ -536,7 +548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>130</v>
       </c>
@@ -548,7 +560,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>140</v>
       </c>
@@ -560,7 +572,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>150</v>
       </c>
@@ -572,7 +584,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>160</v>
       </c>
@@ -873,112 +885,40 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>450</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="0"/>
-        <v>450</v>
-      </c>
+      <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
-        <v>500</v>
-      </c>
-      <c r="C42">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
-        <v>550</v>
-      </c>
-      <c r="C43">
-        <f t="shared" si="0"/>
-        <v>550</v>
-      </c>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>600</v>
-      </c>
-      <c r="C44">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
+      <c r="A44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>650</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="0"/>
-        <v>650</v>
-      </c>
+      <c r="A45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>700</v>
-      </c>
-      <c r="C46">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>750</v>
-      </c>
-      <c r="C47">
-        <f t="shared" si="0"/>
-        <v>750</v>
-      </c>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>800</v>
-      </c>
-      <c r="C48">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>850</v>
-      </c>
-      <c r="C49">
-        <f t="shared" si="0"/>
-        <v>850</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>900</v>
-      </c>
-      <c r="C50">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>950</v>
-      </c>
-      <c r="C51">
-        <f t="shared" si="0"/>
-        <v>950</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>